<commit_message>
Updated script to read multipul channels and save them all seperately.
</commit_message>
<xml_diff>
--- a/Pi_Inventory.xlsx
+++ b/Pi_Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanj\Documents\School\MadLab\RaspberryPi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326F3F36-D166-410B-90B5-7D5903205210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AF62E3-C705-4BCA-9FFA-4F15176D1874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" xr2:uid="{823BD4BA-3DB3-416E-8D49-D956332B067A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" activeTab="2" xr2:uid="{823BD4BA-3DB3-416E-8D49-D956332B067A}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="153">
   <si>
     <t>Working</t>
   </si>
@@ -634,6 +634,9 @@
   </si>
   <si>
     <t>Orientation (sunlight exposure / object distance)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2277,7 +2280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497F7313-7EFD-4A9F-9C42-6D78A8DD5B46}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2776,7 +2779,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2945,6 +2948,11 @@
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="6" t="s">

</xml_diff>